<commit_message>
amélioration plusieurs page excel
</commit_message>
<xml_diff>
--- a/sessions.xlsx
+++ b/sessions.xlsx
@@ -3,21 +3,30 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr date1904="false"/>
   <sheets>
-    <sheet sheetId="1" name="5" r:id="rId4"/>
+    <sheet sheetId="1" name="2ème" r:id="rId4"/>
+    <sheet sheetId="2" name="time.bressani.dev" r:id="rId5"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="6">
     <numFmt numFmtId="100" formatCode="yyyy/mm/dd"/>
     <numFmt numFmtId="101" formatCode="yyyy/mm/dd hh:mm:ss"/>
     <numFmt numFmtId="102" formatCode="dd/mm/yyyy hh:mm:ss"/>
     <numFmt numFmtId="103" formatCode="0.00"/>
+    <numFmt numFmtId="104" formatCode="dd/mm/yyyy hh:mm:ss"/>
+    <numFmt numFmtId="105" formatCode="0.00"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="3">
     <font>
+      <name val="Arial"/>
+      <sz val="11"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b val="1"/>
       <name val="Arial"/>
       <sz val="11"/>
       <family val="1"/>
@@ -37,7 +46,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="10">
     <border/>
     <border>
       <left style="thin">
@@ -50,6 +59,62 @@
         <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
     </border>
@@ -113,7 +178,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" numFmtId="0" fontId="0" fillId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf borderId="0" xfId="0" numFmtId="0" fontId="0" fillId="0"/>
     <xf borderId="1" xfId="0" numFmtId="0" fontId="0" fillId="0"/>
     <xf borderId="0" xfId="0" numFmtId="14" fontId="0" fillId="0" applyNumberFormat="1"/>
@@ -121,6 +186,12 @@
     <xf fillId="0" fontId="0" numFmtId="103" borderId="3" applyFill="0" applyFont="0" applyNumberFormat="1" applyBorder="1" applyAlignment="0" applyProtection="0"/>
     <xf fillId="0" fontId="0" numFmtId="0" borderId="4" applyFill="0" applyFont="0" applyNumberFormat="0" applyBorder="1" applyAlignment="0" applyProtection="0"/>
     <xf fillId="0" fontId="1" numFmtId="0" borderId="5" applyFill="0" applyFont="1" applyNumberFormat="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fillId="0" fontId="0" numFmtId="104" borderId="6" applyFill="0" applyFont="0" applyNumberFormat="1" applyBorder="1" applyAlignment="0" applyProtection="0"/>
+    <xf fillId="0" fontId="0" numFmtId="105" borderId="7" applyFill="0" applyFont="0" applyNumberFormat="1" applyBorder="1" applyAlignment="0" applyProtection="0"/>
+    <xf fillId="0" fontId="0" numFmtId="0" borderId="8" applyFill="0" applyFont="0" applyNumberFormat="0" applyBorder="1" applyAlignment="0" applyProtection="0"/>
+    <xf fillId="0" fontId="2" numFmtId="0" borderId="9" applyFill="0" applyFont="1" applyNumberFormat="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -137,7 +208,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView windowProtection="0" tabSelected="0" showWhiteSpace="0" showOutlineSymbols="0" showFormulas="0" rightToLeft="0" showZeros="1" showRuler="1" showRowColHeaders="1" showGridLines="1" defaultGridColor="1" zoomScale="100" workbookViewId="0" zoomScaleSheetLayoutView="0" zoomScalePageLayoutView="0" zoomScaleNormal="0"/>
   </sheetViews>
@@ -185,17 +256,17 @@
     </row>
     <row r="2">
       <c r="A2" s="5" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B2" s="3">
-        <v>45785.37085648148</v>
+        <v>45784.46271990741</v>
       </c>
       <c r="C2" s="3">
-        <v>45785.370891203704</v>
+        <v>45785.46271990741</v>
       </c>
       <c r="D2" s="5" t="inlineStr">
         <is>
-          <t>00:00:03</t>
+          <t>00:00:00</t>
         </is>
       </c>
       <c r="E2" s="4" t="str">
@@ -203,23 +274,23 @@
       </c>
       <c r="F2" s="5" t="inlineStr">
         <is>
-          <t>essai 1</t>
+          <t>Saisie</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="5" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B3" s="3">
-        <v>45785.371030092596</v>
+        <v>45785.462789351855</v>
       </c>
       <c r="C3" s="3">
-        <v>45785.454363425924</v>
+        <v>45785.4628125</v>
       </c>
       <c r="D3" s="5" t="inlineStr">
         <is>
-          <t>02:00:00</t>
+          <t>00:00:02</t>
         </is>
       </c>
       <c r="E3" s="4" t="str">
@@ -232,156 +303,348 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="5" t="n">
+      <c r="A4" s="5" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="B4" s="5" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="C4" s="5" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="D4" s="5" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="E4" s="5" t="str">
+        <f>SUM(E2:E3)</f>
+      </c>
+      <c r="F4" s="5" t="inlineStr">
+        <is>
+          <t>Total jours</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="5" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="B5" s="5" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="C5" s="5" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="D5" s="5" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="E5" s="5" t="str">
+        <f>E4*8.5</f>
+      </c>
+      <c r="F5" s="5" t="inlineStr">
+        <is>
+          <t>Total heures</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
+  <printOptions verticalCentered="0" horizontalCentered="0" headings="0" gridLines="0"/>
+  <pageMargins right="0.75" left="0.75" bottom="1.0" top="1.0" footer="0.5" header="0.5"/>
+  <pageSetup/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
+  <sheetPr>
+    <pageSetUpPr fitToPage="0"/>
+  </sheetPr>
+  <dimension ref="A1:F10"/>
+  <sheetViews>
+    <sheetView windowProtection="0" tabSelected="0" showWhiteSpace="0" showOutlineSymbols="0" showFormulas="0" rightToLeft="0" showZeros="1" showRuler="1" showRowColHeaders="1" showGridLines="1" defaultGridColor="1" zoomScale="100" workbookViewId="0" zoomScaleSheetLayoutView="0" zoomScalePageLayoutView="0" zoomScaleNormal="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="18"/>
+  <cols>
+    <col min="1" max="1" bestFit="1" customWidth="1" width="6.6"/>
+    <col min="2" max="2" bestFit="1" customWidth="1" width="26.400000000000002"/>
+    <col min="3" max="3" bestFit="1" customWidth="1" width="26.400000000000002"/>
+    <col min="4" max="4" bestFit="1" customWidth="1" width="12.100000000000001"/>
+    <col min="5" max="5" bestFit="1" customWidth="1" width="11.549999999999999"/>
+    <col min="6" max="6" bestFit="1" customWidth="1" width="16.5"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="10" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1" s="10" t="inlineStr">
+        <is>
+          <t>Début</t>
+        </is>
+      </c>
+      <c r="C1" s="10" t="inlineStr">
+        <is>
+          <t>Fin</t>
+        </is>
+      </c>
+      <c r="D1" s="10" t="inlineStr">
+        <is>
+          <t>Durée</t>
+        </is>
+      </c>
+      <c r="E1" s="10" t="inlineStr">
+        <is>
+          <t>Jour travail</t>
+        </is>
+      </c>
+      <c r="F1" s="10" t="inlineStr">
+        <is>
+          <t>Commentaire</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="7">
+        <v>45785.37085648148</v>
+      </c>
+      <c r="C2" s="7">
+        <v>45785.370891203704</v>
+      </c>
+      <c r="D2" s="9" t="inlineStr">
+        <is>
+          <t>00:00:03</t>
+        </is>
+      </c>
+      <c r="E2" s="8" t="str">
+        <f>(C2-B2)*24/8.5</f>
+      </c>
+      <c r="F2" s="9" t="inlineStr">
+        <is>
+          <t>essai 1</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="B3" s="7">
+        <v>45785.371030092596</v>
+      </c>
+      <c r="C3" s="7">
+        <v>45785.454363425924</v>
+      </c>
+      <c r="D3" s="9" t="inlineStr">
+        <is>
+          <t>02:00:00</t>
+        </is>
+      </c>
+      <c r="E3" s="8" t="str">
+        <f>(C3-B3)*24/8.5</f>
+      </c>
+      <c r="F3" s="9" t="inlineStr">
+        <is>
+          <t>Saisie</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="9" t="n">
         <v>2</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="7">
         <v>45785.373773148145</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="7">
         <v>45785.3737962963</v>
       </c>
-      <c r="D4" s="5" t="inlineStr">
+      <c r="D4" s="9" t="inlineStr">
         <is>
           <t>00:00:02</t>
         </is>
       </c>
-      <c r="E4" s="4" t="str">
+      <c r="E4" s="8" t="str">
         <f>(C4-B4)*24/8.5</f>
       </c>
-      <c r="F4" s="5" t="inlineStr">
+      <c r="F4" s="9" t="inlineStr">
         <is>
           <t>essai 2</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="5" t="n">
+      <c r="A5" s="9" t="n">
         <v>3</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="7">
         <v>45785.37384259259</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="7">
         <v>45785.37385416667</v>
       </c>
-      <c r="D5" s="5" t="inlineStr">
+      <c r="D5" s="9" t="inlineStr">
         <is>
           <t>00:00:01</t>
         </is>
       </c>
-      <c r="E5" s="4" t="str">
+      <c r="E5" s="8" t="str">
         <f>(C5-B5)*24/8.5</f>
       </c>
-      <c r="F5" s="5" t="inlineStr">
+      <c r="F5" s="9" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="5" t="n">
+      <c r="A6" s="9" t="n">
         <v>4</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="7">
         <v>45785.37412037037</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="7">
         <v>45785.37553240741</v>
       </c>
-      <c r="D6" s="5" t="inlineStr">
+      <c r="D6" s="9" t="inlineStr">
         <is>
           <t>00:02:02</t>
         </is>
       </c>
-      <c r="E6" s="4" t="str">
+      <c r="E6" s="8" t="str">
         <f>(C6-B6)*24/8.5</f>
       </c>
-      <c r="F6" s="5" t="inlineStr">
+      <c r="F6" s="9" t="inlineStr">
         <is>
           <t>Long</t>
         </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="5" t="n">
+      <c r="A7" s="9" t="n">
         <v>5</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="7">
         <v>45785.37574074074</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="7">
         <v>45785.375810185185</v>
       </c>
-      <c r="D7" s="5" t="inlineStr">
+      <c r="D7" s="9" t="inlineStr">
         <is>
           <t>00:00:06</t>
         </is>
       </c>
-      <c r="E7" s="4" t="str">
+      <c r="E7" s="8" t="str">
         <f>(C7-B7)*24/8.5</f>
       </c>
-      <c r="F7" s="5" t="inlineStr">
+      <c r="F7" s="9" t="inlineStr">
         <is>
           <t>plus long</t>
         </is>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="5" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="B8" s="5" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="C8" s="5" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="D8" s="5" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="E8" s="5" t="str">
-        <f>SUM(E2:E7)</f>
-      </c>
-      <c r="F8" s="5" t="inlineStr">
+      <c r="A8" s="9" t="n">
+        <v>9</v>
+      </c>
+      <c r="B8" s="7">
+        <v>45785.463425925926</v>
+      </c>
+      <c r="C8" s="7">
+        <v>45785.4634375</v>
+      </c>
+      <c r="D8" s="9" t="inlineStr">
+        <is>
+          <t>00:00:01</t>
+        </is>
+      </c>
+      <c r="E8" s="8" t="str">
+        <f>(C8-B8)*24/8.5</f>
+      </c>
+      <c r="F8" s="9" t="inlineStr">
+        <is>
+          <t>fin</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="9" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="B9" s="9" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="C9" s="9" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="D9" s="9" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="E9" s="9" t="str">
+        <f>SUM(E2:E8)</f>
+      </c>
+      <c r="F9" s="9" t="inlineStr">
         <is>
           <t>Total jours</t>
         </is>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" s="5" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="B9" s="5" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="C9" s="5" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="D9" s="5" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="E9" s="5" t="str">
-        <f>E8*8.5</f>
-      </c>
-      <c r="F9" s="5" t="inlineStr">
+    <row r="10">
+      <c r="A10" s="9" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="B10" s="9" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="C10" s="9" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="D10" s="9" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="E10" s="9" t="str">
+        <f>E9*8.5</f>
+      </c>
+      <c r="F10" s="9" t="inlineStr">
         <is>
           <t>Total heures</t>
         </is>

</xml_diff>